<commit_message>
update testcase cua Huong
</commit_message>
<xml_diff>
--- a/TestCase_Nhom10.xlsx
+++ b/TestCase_Nhom10.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\OneDrive - TRƯỜNG ĐẠI HỌC MỞ TP.HCM\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66543FCE-34EC-45C8-83C6-7BE756CDE178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C3E5D2C-D2D2-4D22-ACA5-E52AEB9C049E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="821" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="821" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="97" r:id="rId1"/>
@@ -31,11 +31,22 @@
     <definedName name="VancoProducts">[1]Validation!$B$2:$B$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="76">
   <si>
     <t>TC1</t>
   </si>
@@ -203,6 +214,9 @@
     <t>Test Leader 01</t>
   </si>
   <si>
+    <t>Sample Project</t>
+  </si>
+  <si>
     <t>CR100 - Export to excel</t>
   </si>
   <si>
@@ -218,365 +232,335 @@
     <t>DeviceManagementSystem</t>
   </si>
   <si>
-    <t>DMS1.0</t>
-  </si>
-  <si>
-    <t>Lê Hữu Hậu</t>
-  </si>
-  <si>
-    <t>Kiểm tra chức năng đăng nhập (Admin) với tài khoản và mật khẩu hợp lệ</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Hiển thị danh sách </t>
+    <t>###</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kiểm tra đăng nhập thành công bằng tài khoản và mật khẩu hợp lệ </t>
+  </si>
+  <si>
+    <t>Actual Results</t>
+  </si>
+  <si>
+    <t>1. Kiểm tra chức năng đăng nhập HỢP LỆ</t>
+  </si>
+  <si>
+    <t>1. Kiểm tra chức năng đăng nhập KHÔNG HỢP LỆ</t>
+  </si>
+  <si>
+    <t>TC4</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>1. Vào trang đăng nhập 
+2. Nhấn login</t>
+  </si>
+  <si>
+    <t>Nội dung thông báo chưa rõ ràng!!!</t>
+  </si>
+  <si>
+    <t>Hiện ra trang Danh sách thiết bị</t>
+  </si>
+  <si>
+    <t>TC5</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Vào trang đăng nhập 
+2. Nhập "username" tồn tại trong hệ thống : </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="10"/>
         <color rgb="FF000000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
-      <t>thiết bị</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Kiểm tra chức năng đăng nhập </t>
+      <t>lehuuhau</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+3. Nhập "password" có 8 ký tự hợp lệ: </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="10"/>
         <color rgb="FF000000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
-      <t>thành công</t>
+      <t>Lehuuhau1231@</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
         <color indexed="8"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
-      <t xml:space="preserve"> với tài khoản và mật khẩu </t>
+      <t xml:space="preserve">
+4. Nhấn login
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Kiểm tra đăng nhập không thành công </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="10"/>
         <color rgb="FF000000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
-      <t>hợp lệ</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Đăng nhập </t>
+      <t>bằng tài khoản không tồn tại trong hệ thống</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Vào trang đăng nhập 
+2. Nhập "username" không tồn tại trong hệ thống : </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="10"/>
         <color rgb="FF000000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
-      <t>thất bại</t>
+      <t>abc123</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
-      <t>. Hiển thị thông báo "Sai tài khoản hoặc mật khẩu"</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>Đăng nhập</t>
+      <t xml:space="preserve">
+3. Nhập "password" có 8 ký tự hợp lệ: </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="10"/>
         <color rgb="FF000000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
-      <t xml:space="preserve"> thất bại</t>
+      <t>Abc1231@</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
-      <t>. Hiển thị thông báo "Sai tài khoản hoặc mật khẩu"</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1: Truy cập vào </t>
+      <t xml:space="preserve">
+4. Nhấn login</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Hiện thông báo tài khoản</t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="10"/>
         <color rgb="FF000000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
-      <t>phần mềm</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-2: Nhập </t>
+      <t xml:space="preserve"> Không tồn tại trong hệ thống</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Kiểm tra đăng nhập không thành công </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="10"/>
         <color rgb="FF000000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
-      <t>đúng</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> với tên tài khoản: "admin"
-3: Nhập </t>
+      <t>bằng mật khẩu không hợp lệ</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Vào trang đăng nhập 
+2. Nhập "username" tồn tại trong hệ thống : </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="10"/>
         <color rgb="FF000000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
-      <t>đúng</t>
+      <t>lehuuhau</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
         <color indexed="8"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
-      <t xml:space="preserve"> với mật khẩu: "admin123"
-4: </t>
+      <t xml:space="preserve">
+3. Nhập "password" không hợp lệ : </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="10"/>
         <color rgb="FF000000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
-      <t>Click</t>
+      <t>Abc1231@</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
         <color indexed="8"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
-      <t xml:space="preserve"> vào nút đăng nhập</t>
-    </r>
-  </si>
-  <si>
-    <t>Kiểm tra chức năng đăng nhập (Admin) với tài khoản không hợp lệ</t>
-  </si>
-  <si>
-    <t>Kiểm tra chức năng đăng nhập (Admin) với mật khẩu không hợp lệ</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Kiểm tra chức năng đăng nhập </t>
+      <t xml:space="preserve">
+4. Nhấn login</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Hiện thông báo</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Sai mật khẩu hoặc tài khoản</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Kiểm tra đăng nhập không thành công </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="10"/>
         <color rgb="FF000000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
-      <t>thất bại</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> với tài khoản </t>
+      <t>khi bỏ trống "username" và "password"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Hiện thông báo</t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="10"/>
         <color rgb="FF000000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
-      <t>không hợp lệ</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Kiểm tra chức năng đăng nhập </t>
+      <t xml:space="preserve"> Chưa nhập username</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Kiểm tra đăng nhập không thành công </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="10"/>
         <color rgb="FF000000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
-      <t>thất bại</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> với mật khẩu </t>
+      <t>bằng mật khẩu bỏ trống</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Vào trang đăng nhập 
+2. Nhập "username" tồn tại trong hệ thống : </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="10"/>
         <color rgb="FF000000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
-      <t>không hợp lệ</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1: Truy cập vào </t>
+      <t>lehuuhau</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+3. Không nhập password
+4. Nhấn login</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Hiện thông báo</t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
-      <t>phần mềm</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-2: Nhập với tên tài khoản: "z"
-3: Nhập với mật khẩu: "admin123"
-4: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>Click</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> vào nút đăng nhập</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1: Truy cập vào </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>phần mềm</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-2: Nhập với tên tài khoản: "admin"
-3: Nhập với mật khẩu: "aaa"
-4: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>Click</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> vào nút đăng nhập</t>
+      <t xml:space="preserve"> Chưa nhập password</t>
     </r>
   </si>
 </sst>
@@ -588,7 +572,7 @@
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -722,39 +706,45 @@
       <b/>
       <sz val="10"/>
       <color indexed="8"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <color indexed="10"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF00B050"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF00B050"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -795,7 +785,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -1167,17 +1157,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -1253,6 +1232,43 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -1367,6 +1383,18 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="15" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1450,18 +1478,6 @@
     <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1479,11 +1495,110 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="4" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1491,156 +1606,57 @@
     <xf numFmtId="0" fontId="22" fillId="4" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="25" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="23" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="23" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="27" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_Functional Test Case v1.0" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal_Sheet1_Vanco_CR022a1_TestCase_v0.1" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="標準_結合試験(AllOvertheWorld)" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
@@ -1656,6 +1672,231 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>56744</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>40532</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2814734</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>1563809</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Hình ảnh 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D477F5BD-FA42-B4B7-1FC7-B3A794164287}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8081071" y="2303205"/>
+          <a:ext cx="2757990" cy="1523277"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>108857</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>23326</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2760306</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>1586204</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Hình ảnh 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F315CDC-CA08-F47B-1192-C232BA81F8D3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8475306" y="4128795"/>
+          <a:ext cx="2651449" cy="1562878"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>25831</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>27363</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2736273</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>1498023</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Hình ảnh 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02188356-80B1-580E-8AB0-43A5C9AED777}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8710899" y="7326977"/>
+          <a:ext cx="2710442" cy="1470660"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>60615</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>69272</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2788229</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>1489363</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Hình ảnh 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35DA3CCE-1A14-A7A9-0DF5-DD0306B7E427}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8745683" y="5749636"/>
+          <a:ext cx="2727614" cy="1420091"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>51955</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2770908</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>1604496</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Hình ảnh 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C45826E-37F3-1A38-8E38-DB54A42D3494}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8780318" y="8918864"/>
+          <a:ext cx="2675658" cy="1552541"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1961,23 +2202,23 @@
   <dimension ref="A2:H23"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="14.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="1"/>
     <col min="4" max="4" width="15" style="1" customWidth="1"/>
-    <col min="5" max="5" width="32.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="23.875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="26.625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.77734375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.44140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="26.6640625" style="1" customWidth="1"/>
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="22.5">
+    <row r="2" spans="1:8" ht="22.2">
       <c r="A2" s="25"/>
       <c r="B2" s="26" t="s">
         <v>5</v>
@@ -1993,8 +2234,8 @@
       <c r="B3" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="57">
-        <v>1.1000000000000001</v>
+      <c r="C3" s="61">
+        <v>1.2</v>
       </c>
       <c r="D3" s="28"/>
       <c r="E3" s="25"/>
@@ -2006,15 +2247,15 @@
       <c r="B4" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="11">
-        <v>45739</v>
+      <c r="C4" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="25"/>
       <c r="F4" s="25"/>
       <c r="G4" s="25"/>
     </row>
-    <row r="5" spans="1:8" ht="15" thickBot="1">
+    <row r="5" spans="1:8" ht="14.4" thickBot="1">
       <c r="A5" s="25"/>
       <c r="B5" s="27"/>
       <c r="C5" s="28"/>
@@ -2028,11 +2269,11 @@
       <c r="B6" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="101" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="101"/>
-      <c r="E6" s="102"/>
+      <c r="C6" s="92" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="92"/>
+      <c r="E6" s="93"/>
       <c r="F6" s="25"/>
       <c r="G6" s="25"/>
     </row>
@@ -2041,11 +2282,9 @@
       <c r="B7" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="101" t="s">
-        <v>52</v>
-      </c>
-      <c r="D7" s="101"/>
-      <c r="E7" s="102"/>
+      <c r="C7" s="92"/>
+      <c r="D7" s="92"/>
+      <c r="E7" s="93"/>
       <c r="F7" s="25"/>
       <c r="G7" s="25"/>
     </row>
@@ -2072,32 +2311,32 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="34" customFormat="1" ht="25.5">
-      <c r="B11" s="46" t="s">
+    <row r="11" spans="1:8" s="34" customFormat="1" ht="26.4">
+      <c r="B11" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="47" t="s">
+      <c r="C11" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="47" t="s">
+      <c r="D11" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="47" t="s">
+      <c r="E11" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="47" t="s">
+      <c r="F11" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="48" t="s">
+      <c r="G11" s="52" t="s">
         <v>14</v>
       </c>
       <c r="H11" s="82" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="34" customFormat="1">
+    <row r="12" spans="1:8" s="34" customFormat="1" ht="26.4">
       <c r="B12" s="36">
-        <v>45739</v>
+        <v>39293</v>
       </c>
       <c r="C12" s="37" t="s">
         <v>41</v>
@@ -2106,31 +2345,57 @@
       <c r="E12" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="69" t="s">
-        <v>53</v>
+      <c r="F12" s="73" t="s">
+        <v>50</v>
       </c>
       <c r="G12" s="81"/>
-      <c r="H12" s="83"/>
-    </row>
-    <row r="13" spans="1:8" s="34" customFormat="1">
-      <c r="B13" s="98"/>
-      <c r="C13" s="99"/>
-      <c r="D13" s="99"/>
-      <c r="E13" s="99"/>
-      <c r="F13" s="99"/>
-      <c r="G13" s="99"/>
-      <c r="H13" s="45"/>
-    </row>
-    <row r="14" spans="1:8" s="35" customFormat="1" ht="12.75">
-      <c r="B14" s="100"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="42"/>
-    </row>
-    <row r="15" spans="1:8" s="35" customFormat="1" ht="12.75">
+      <c r="H12" s="83" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="34" customFormat="1" ht="26.4">
+      <c r="B13" s="89">
+        <v>39295</v>
+      </c>
+      <c r="C13" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="38"/>
+      <c r="E13" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="73" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" s="88" t="s">
+        <v>51</v>
+      </c>
+      <c r="H13" s="83" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="35" customFormat="1" ht="26.4">
+      <c r="B14" s="36">
+        <v>39311</v>
+      </c>
+      <c r="C14" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="38"/>
+      <c r="E14" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="73" t="s">
+        <v>50</v>
+      </c>
+      <c r="G14" s="88" t="s">
+        <v>46</v>
+      </c>
+      <c r="H14" s="83" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="35" customFormat="1" ht="13.2">
       <c r="B15" s="43"/>
       <c r="C15" s="44"/>
       <c r="D15" s="41"/>
@@ -2194,46 +2459,22 @@
       <c r="H21" s="42"/>
     </row>
     <row r="22" spans="2:8" s="34" customFormat="1">
-      <c r="B22" s="93">
-        <v>39295</v>
-      </c>
-      <c r="C22" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22" s="38"/>
-      <c r="E22" s="39" t="s">
-        <v>44</v>
-      </c>
-      <c r="F22" s="69" t="s">
-        <v>49</v>
-      </c>
-      <c r="G22" s="92" t="s">
-        <v>50</v>
-      </c>
-      <c r="H22" s="83" t="s">
-        <v>42</v>
-      </c>
+      <c r="B22" s="43"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="41"/>
+      <c r="G22" s="41"/>
+      <c r="H22" s="42"/>
     </row>
     <row r="23" spans="2:8" s="34" customFormat="1">
-      <c r="B23" s="36">
-        <v>39311</v>
-      </c>
-      <c r="C23" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" s="38"/>
-      <c r="E23" s="39" t="s">
-        <v>44</v>
-      </c>
-      <c r="F23" s="69" t="s">
-        <v>49</v>
-      </c>
-      <c r="G23" s="92" t="s">
-        <v>46</v>
-      </c>
-      <c r="H23" s="83" t="s">
-        <v>42</v>
-      </c>
+      <c r="B23" s="46"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="48"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2254,343 +2495,401 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:K55"/>
+  <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="15.625" customWidth="1"/>
-    <col min="2" max="2" width="18.125" customWidth="1"/>
-    <col min="3" max="3" width="42.125" customWidth="1"/>
-    <col min="6" max="6" width="23.625" customWidth="1"/>
-    <col min="7" max="7" width="18.5" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="17.125" customWidth="1"/>
-    <col min="9" max="9" width="9" style="87"/>
-    <col min="10" max="10" width="18" style="86" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" customWidth="1"/>
+    <col min="3" max="3" width="51.6640625" customWidth="1"/>
+    <col min="6" max="6" width="23.6640625" customWidth="1"/>
+    <col min="7" max="7" width="18.44140625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="41.21875" customWidth="1"/>
+    <col min="9" max="9" width="17.109375" customWidth="1"/>
+    <col min="10" max="10" width="9" style="87"/>
+    <col min="11" max="11" width="18" style="86" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A1" s="58" t="s">
+    <row r="1" spans="1:12" s="2" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A1" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="107"/>
-      <c r="D1" s="107"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
-      <c r="I1" s="94"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="7"/>
-    </row>
-    <row r="2" spans="1:11" s="2" customFormat="1" ht="11.25" customHeight="1" thickBot="1">
+      <c r="I1" s="6"/>
+      <c r="J1" s="90"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="7"/>
+    </row>
+    <row r="2" spans="1:12" s="2" customFormat="1" ht="11.25" customHeight="1" thickBot="1">
       <c r="A2" s="7"/>
-      <c r="B2" s="108"/>
-      <c r="C2" s="108"/>
-      <c r="D2" s="108"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
-      <c r="I2" s="94"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="76"/>
-    </row>
-    <row r="3" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
-      <c r="A3" s="59" t="s">
+      <c r="I2" s="6"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="7"/>
+    </row>
+    <row r="3" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1">
+      <c r="A3" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="101" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" s="101"/>
-      <c r="D3" s="102"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="117"/>
-      <c r="I3" s="117"/>
-      <c r="J3" s="117"/>
-      <c r="K3" s="9"/>
-    </row>
-    <row r="4" spans="1:11" s="3" customFormat="1" ht="12.75">
-      <c r="A4" s="64" t="s">
+      <c r="B3" s="102" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="103"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="101"/>
+      <c r="J3" s="101"/>
+      <c r="K3" s="101"/>
+      <c r="L3" s="9"/>
+    </row>
+    <row r="4" spans="1:12" s="3" customFormat="1" ht="13.2">
+      <c r="A4" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="118" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="119"/>
-      <c r="D4" s="120"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="117"/>
-      <c r="I4" s="117"/>
-      <c r="J4" s="117"/>
-      <c r="K4" s="9"/>
-    </row>
-    <row r="5" spans="1:11" s="73" customFormat="1" ht="12.75">
-      <c r="A5" s="64" t="s">
+      <c r="B4" s="107" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="108"/>
+      <c r="D4" s="109"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="101"/>
+      <c r="J4" s="101"/>
+      <c r="K4" s="101"/>
+      <c r="L4" s="9"/>
+    </row>
+    <row r="5" spans="1:12" s="77" customFormat="1" ht="26.4">
+      <c r="A5" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="110" t="s">
-        <v>48</v>
-      </c>
-      <c r="C5" s="111"/>
-      <c r="D5" s="112"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="116"/>
-      <c r="I5" s="116"/>
-      <c r="J5" s="116"/>
-      <c r="K5" s="72"/>
-    </row>
-    <row r="6" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
+      <c r="B5" s="97" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="98"/>
+      <c r="D5" s="99"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="75"/>
+      <c r="I5" s="100"/>
+      <c r="J5" s="100"/>
+      <c r="K5" s="100"/>
+      <c r="L5" s="76"/>
+    </row>
+    <row r="6" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A6" s="12" t="s">
         <v>39</v>
       </c>
       <c r="B6" s="84">
-        <f>COUNTIF(I12:I17,"Pass")</f>
-        <v>3</v>
+        <f>COUNTIF(J12:J18,"Pass")</f>
+        <v>4</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>40</v>
       </c>
       <c r="D6" s="13">
-        <f>COUNTIF(I10:I736,"Pending")</f>
+        <f>COUNTIF(J10:J733,"Pending")</f>
         <v>0</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="117"/>
-      <c r="I6" s="117"/>
-      <c r="J6" s="117"/>
-      <c r="K6" s="9"/>
-    </row>
-    <row r="7" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1">
+      <c r="H6" s="8"/>
+      <c r="I6" s="101"/>
+      <c r="J6" s="101"/>
+      <c r="K6" s="101"/>
+      <c r="L6" s="9"/>
+    </row>
+    <row r="7" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1">
       <c r="A7" s="14" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="85">
-        <f>COUNTIF(I12:I17,"Fail")</f>
+        <f>COUNTIF(J12:J18,"Fail")</f>
         <v>0</v>
       </c>
       <c r="C7" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="60">
-        <f>COUNTA(A12:A17) -15</f>
-        <v>-9</v>
-      </c>
-      <c r="E7" s="63"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="63"/>
-      <c r="H7" s="117"/>
-      <c r="I7" s="117"/>
-      <c r="J7" s="117"/>
-      <c r="K7" s="9"/>
-    </row>
-    <row r="8" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="109"/>
-      <c r="B8" s="109"/>
-      <c r="C8" s="109"/>
-      <c r="D8" s="109"/>
+      <c r="D7" s="64">
+        <f>COUNTA(A12:A18) -15</f>
+        <v>-8</v>
+      </c>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="67"/>
+      <c r="I7" s="101"/>
+      <c r="J7" s="101"/>
+      <c r="K7" s="101"/>
+      <c r="L7" s="9"/>
+    </row>
+    <row r="8" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1">
+      <c r="A8" s="96"/>
+      <c r="B8" s="96"/>
+      <c r="C8" s="96"/>
+      <c r="D8" s="96"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
-      <c r="I8" s="95"/>
-      <c r="J8" s="95"/>
-      <c r="K8" s="9"/>
-    </row>
-    <row r="9" spans="1:11" s="75" customFormat="1" ht="12" customHeight="1">
-      <c r="A9" s="125" t="s">
+      <c r="I8" s="8"/>
+      <c r="J8" s="91"/>
+      <c r="K8" s="91"/>
+      <c r="L8" s="9"/>
+    </row>
+    <row r="9" spans="1:12" s="79" customFormat="1" ht="12" customHeight="1">
+      <c r="A9" s="105" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="126" t="s">
+      <c r="B9" s="112" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="125" t="s">
+      <c r="C9" s="105" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="128" t="s">
+      <c r="D9" s="115" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="129"/>
-      <c r="F9" s="129"/>
-      <c r="G9" s="130"/>
-      <c r="H9" s="121" t="s">
+      <c r="E9" s="116"/>
+      <c r="F9" s="116"/>
+      <c r="G9" s="117"/>
+      <c r="H9" s="114" t="s">
+        <v>55</v>
+      </c>
+      <c r="I9" s="105" t="s">
         <v>28</v>
       </c>
-      <c r="I9" s="103" t="s">
+      <c r="J9" s="105" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="103" t="s">
+      <c r="K9" s="105" t="s">
         <v>33</v>
       </c>
-      <c r="K9" s="74"/>
-    </row>
-    <row r="10" spans="1:11" s="3" customFormat="1" ht="12" customHeight="1">
-      <c r="A10" s="103"/>
-      <c r="B10" s="127"/>
-      <c r="C10" s="103"/>
-      <c r="D10" s="122"/>
-      <c r="E10" s="131"/>
-      <c r="F10" s="131"/>
-      <c r="G10" s="132"/>
-      <c r="H10" s="122"/>
-      <c r="I10" s="103"/>
-      <c r="J10" s="103"/>
-      <c r="K10" s="9"/>
-    </row>
-    <row r="11" spans="1:11" s="76" customFormat="1" ht="15">
-      <c r="A11" s="123"/>
-      <c r="B11" s="123"/>
-      <c r="C11" s="123"/>
-      <c r="D11" s="123"/>
-      <c r="E11" s="123"/>
-      <c r="F11" s="123"/>
-      <c r="G11" s="123"/>
-      <c r="H11" s="123"/>
-      <c r="I11" s="123"/>
-      <c r="J11" s="124"/>
-    </row>
-    <row r="12" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A12" s="113" t="s">
+      <c r="L9" s="78"/>
+    </row>
+    <row r="10" spans="1:12" s="3" customFormat="1" ht="12" customHeight="1">
+      <c r="A10" s="106"/>
+      <c r="B10" s="113"/>
+      <c r="C10" s="106"/>
+      <c r="D10" s="118"/>
+      <c r="E10" s="119"/>
+      <c r="F10" s="119"/>
+      <c r="G10" s="120"/>
+      <c r="H10" s="106"/>
+      <c r="I10" s="106"/>
+      <c r="J10" s="106"/>
+      <c r="K10" s="106"/>
+      <c r="L10" s="9"/>
+    </row>
+    <row r="11" spans="1:12" s="80" customFormat="1" ht="15">
+      <c r="A11" s="110"/>
+      <c r="B11" s="110"/>
+      <c r="C11" s="110"/>
+      <c r="D11" s="110"/>
+      <c r="E11" s="110"/>
+      <c r="F11" s="110"/>
+      <c r="G11" s="110"/>
+      <c r="H11" s="110"/>
+      <c r="I11" s="110"/>
+      <c r="J11" s="110"/>
+      <c r="K11" s="111"/>
+    </row>
+    <row r="12" spans="1:12" s="4" customFormat="1" ht="13.2">
+      <c r="A12" s="122" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="123"/>
+      <c r="C12" s="123"/>
+      <c r="D12" s="123"/>
+      <c r="E12" s="123"/>
+      <c r="F12" s="123"/>
+      <c r="G12" s="123"/>
+      <c r="H12" s="123"/>
+      <c r="I12" s="123"/>
+      <c r="J12" s="123"/>
+      <c r="K12" s="124"/>
+    </row>
+    <row r="13" spans="1:12" s="4" customFormat="1" ht="130.80000000000001" customHeight="1" outlineLevel="1">
+      <c r="A13" s="125" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="126" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="114"/>
-      <c r="C12" s="114"/>
-      <c r="D12" s="114"/>
-      <c r="E12" s="114"/>
-      <c r="F12" s="114"/>
-      <c r="G12" s="114"/>
-      <c r="H12" s="114"/>
-      <c r="I12" s="114"/>
-      <c r="J12" s="115"/>
-    </row>
-    <row r="13" spans="1:11" s="4" customFormat="1" ht="51" outlineLevel="1">
-      <c r="A13" s="80" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="96" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" s="79" t="s">
+      <c r="C13" s="127" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="128" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="129"/>
+      <c r="F13" s="129"/>
+      <c r="G13" s="130"/>
+      <c r="H13" s="131"/>
+      <c r="I13" s="132">
+        <v>45740</v>
+      </c>
+      <c r="J13" s="133" t="s">
+        <v>39</v>
+      </c>
+      <c r="K13" s="134"/>
+    </row>
+    <row r="14" spans="1:12" s="4" customFormat="1" ht="15" customHeight="1" outlineLevel="1">
+      <c r="A14" s="122" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="123"/>
+      <c r="C14" s="123"/>
+      <c r="D14" s="123"/>
+      <c r="E14" s="123"/>
+      <c r="F14" s="123"/>
+      <c r="G14" s="123"/>
+      <c r="H14" s="123"/>
+      <c r="I14" s="123"/>
+      <c r="J14" s="123"/>
+      <c r="K14" s="124"/>
+    </row>
+    <row r="15" spans="1:12" ht="127.8" customHeight="1">
+      <c r="A15" s="125" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="135" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="135" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="136" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="137"/>
+      <c r="F15" s="137"/>
+      <c r="G15" s="130"/>
+      <c r="H15" s="131"/>
+      <c r="I15" s="138">
+        <v>45741</v>
+      </c>
+      <c r="J15" s="139" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="106" t="s">
-        <v>55</v>
-      </c>
-      <c r="E13" s="105"/>
-      <c r="F13" s="105"/>
-      <c r="G13" s="78"/>
-      <c r="H13" s="133">
-        <v>45740</v>
-      </c>
-      <c r="I13" s="134" t="s">
+      <c r="K15" s="134" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="127.8" customHeight="1">
+      <c r="A16" s="125" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="127" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="127" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="140" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" s="137"/>
+      <c r="F16" s="137"/>
+      <c r="G16" s="130"/>
+      <c r="H16" s="131"/>
+      <c r="I16" s="138">
+        <v>45741</v>
+      </c>
+      <c r="J16" s="133" t="s">
         <v>39</v>
       </c>
-      <c r="J13" s="77"/>
-    </row>
-    <row r="14" spans="1:11" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A14" s="136" t="s">
+      <c r="K16" s="134"/>
+    </row>
+    <row r="17" spans="1:11" ht="123.6" customHeight="1">
+      <c r="A17" s="125" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="135" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="135" t="s">
         <v>60</v>
       </c>
-      <c r="B14" s="137"/>
-      <c r="C14" s="137"/>
-      <c r="D14" s="90"/>
-      <c r="E14" s="90"/>
-      <c r="F14" s="90"/>
-      <c r="G14" s="90"/>
-      <c r="H14" s="97"/>
-      <c r="I14" s="135"/>
-      <c r="J14" s="91"/>
-    </row>
-    <row r="15" spans="1:11" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
-      <c r="A15" s="80" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="88" t="s">
-        <v>62</v>
-      </c>
-      <c r="C15" s="89" t="s">
-        <v>64</v>
-      </c>
-      <c r="D15" s="138" t="s">
-        <v>57</v>
-      </c>
-      <c r="E15" s="105"/>
-      <c r="F15" s="105"/>
-      <c r="G15" s="78"/>
-      <c r="H15" s="139">
-        <v>45740</v>
-      </c>
-      <c r="I15" s="134" t="s">
+      <c r="D17" s="136" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" s="137"/>
+      <c r="F17" s="137"/>
+      <c r="G17" s="130"/>
+      <c r="H17" s="131"/>
+      <c r="I17" s="138">
+        <v>45741</v>
+      </c>
+      <c r="J17" s="133" t="s">
         <v>39</v>
       </c>
-      <c r="J15" s="77"/>
-    </row>
-    <row r="16" spans="1:11" s="4" customFormat="1" ht="12.75" customHeight="1" outlineLevel="1">
-      <c r="A16" s="136" t="s">
-        <v>61</v>
-      </c>
-      <c r="B16" s="137"/>
-      <c r="C16" s="137"/>
-      <c r="D16" s="90"/>
-      <c r="E16" s="90"/>
-      <c r="F16" s="90"/>
-      <c r="G16" s="90"/>
-      <c r="H16" s="97"/>
-      <c r="I16" s="135"/>
-      <c r="J16" s="91"/>
-    </row>
-    <row r="17" spans="1:10" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
-      <c r="A17" s="80" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="96" t="s">
+      <c r="K17" s="134"/>
+    </row>
+    <row r="18" spans="1:11" ht="130.80000000000001" customHeight="1">
+      <c r="A18" s="125" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="79" t="s">
-        <v>65</v>
-      </c>
-      <c r="D17" s="140" t="s">
-        <v>58</v>
-      </c>
-      <c r="E17" s="104"/>
-      <c r="F17" s="104"/>
-      <c r="G17" s="78"/>
-      <c r="H17" s="139">
-        <v>45740</v>
-      </c>
-      <c r="I17" s="134" t="s">
+      <c r="B18" s="127" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="127" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" s="140" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" s="137"/>
+      <c r="F18" s="137"/>
+      <c r="G18" s="130"/>
+      <c r="H18" s="131"/>
+      <c r="I18" s="138">
+        <v>45741</v>
+      </c>
+      <c r="J18" s="133" t="s">
         <v>39</v>
       </c>
-      <c r="J17" s="77"/>
-    </row>
-    <row r="18" spans="1:10" ht="12" customHeight="1"/>
-    <row r="19" spans="1:10" ht="12" customHeight="1"/>
-    <row r="20" spans="1:10" ht="12" customHeight="1"/>
-    <row r="21" spans="1:10" ht="12" customHeight="1"/>
-    <row r="22" spans="1:10" ht="12" customHeight="1"/>
-    <row r="23" spans="1:10" ht="12" customHeight="1"/>
-    <row r="24" spans="1:10" ht="12" customHeight="1"/>
-    <row r="25" spans="1:10" ht="12" customHeight="1"/>
-    <row r="26" spans="1:10" ht="12" customHeight="1"/>
-    <row r="27" spans="1:10" ht="12" customHeight="1"/>
-    <row r="28" spans="1:10" ht="12" customHeight="1"/>
-    <row r="29" spans="1:10" ht="12" customHeight="1"/>
-    <row r="30" spans="1:10" ht="12" customHeight="1"/>
-    <row r="31" spans="1:10" ht="12" customHeight="1"/>
-    <row r="32" spans="1:10" ht="12" customHeight="1"/>
+      <c r="K18" s="134"/>
+    </row>
+    <row r="19" spans="1:11" ht="12" customHeight="1">
+      <c r="E19" s="121"/>
+    </row>
+    <row r="20" spans="1:11" ht="12" customHeight="1"/>
+    <row r="21" spans="1:11" ht="12" customHeight="1"/>
+    <row r="22" spans="1:11" ht="12" customHeight="1"/>
+    <row r="23" spans="1:11" ht="12" customHeight="1"/>
+    <row r="24" spans="1:11" ht="12" customHeight="1"/>
+    <row r="25" spans="1:11" ht="12" customHeight="1"/>
+    <row r="26" spans="1:11" ht="12" customHeight="1"/>
+    <row r="27" spans="1:11" ht="12" customHeight="1"/>
+    <row r="28" spans="1:11" ht="12" customHeight="1"/>
+    <row r="29" spans="1:11" ht="12" customHeight="1"/>
+    <row r="30" spans="1:11" ht="12" customHeight="1"/>
+    <row r="31" spans="1:11" ht="12" customHeight="1"/>
+    <row r="32" spans="1:11" ht="12" customHeight="1"/>
     <row r="33" ht="12" customHeight="1"/>
     <row r="34" ht="12" customHeight="1"/>
     <row r="35" ht="12" customHeight="1"/>
@@ -2608,43 +2907,40 @@
     <row r="47" ht="12" customHeight="1"/>
     <row r="48" ht="12" customHeight="1"/>
     <row r="49" ht="12" customHeight="1"/>
-    <row r="50" ht="12" customHeight="1"/>
-    <row r="51" ht="12" customHeight="1"/>
-    <row r="52" ht="12" customHeight="1"/>
-    <row r="53" ht="12" customHeight="1"/>
-    <row r="54" ht="12" customHeight="1"/>
-    <row r="55" ht="12" customHeight="1"/>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="B1:D2"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="H4:J4"/>
+  <mergeCells count="26">
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="A14:K14"/>
+    <mergeCell ref="D18:F18"/>
     <mergeCell ref="J9:J10"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="D17:F17"/>
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="D13:F13"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D9:G10"/>
-    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="B1:D2"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="A12:K12"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="A11:K11"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2653,16 +2949,16 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2"/>
   <cols>
-    <col min="3" max="3" width="22.875" customWidth="1"/>
-    <col min="7" max="7" width="18.875" customWidth="1"/>
+    <col min="3" max="3" width="22.77734375" customWidth="1"/>
+    <col min="7" max="7" width="18.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="22.5">
+    <row r="1" spans="1:7" ht="22.2">
       <c r="A1" s="15" t="s">
         <v>11</v>
       </c>
@@ -2682,7 +2978,7 @@
       <c r="F2" s="17"/>
       <c r="G2" s="18"/>
     </row>
-    <row r="3" spans="1:7" ht="14.25">
+    <row r="3" spans="1:7" ht="13.8">
       <c r="B3" s="19" t="s">
         <v>10</v>
       </c>
@@ -2692,17 +2988,17 @@
       <c r="F3" s="17"/>
       <c r="G3" s="18"/>
     </row>
-    <row r="4" spans="1:7" ht="14.25">
+    <row r="4" spans="1:7" ht="13.8">
       <c r="B4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="93"/>
+      <c r="C4" s="89"/>
       <c r="D4" s="19"/>
       <c r="E4" s="19"/>
       <c r="F4" s="19"/>
       <c r="G4" s="19"/>
     </row>
-    <row r="5" spans="1:7" ht="14.25">
+    <row r="5" spans="1:7" ht="13.8">
       <c r="A5" s="19"/>
       <c r="B5" s="19"/>
       <c r="C5" s="19"/>
@@ -2711,7 +3007,7 @@
       <c r="F5" s="19"/>
       <c r="G5" s="19"/>
     </row>
-    <row r="6" spans="1:7" ht="14.25">
+    <row r="6" spans="1:7" ht="13.8">
       <c r="A6" s="19"/>
       <c r="B6" s="19"/>
       <c r="C6" s="19"/>
@@ -2720,86 +3016,86 @@
       <c r="F6" s="19"/>
       <c r="G6" s="19"/>
     </row>
-    <row r="7" spans="1:7" ht="14.25">
+    <row r="7" spans="1:7" ht="26.4">
       <c r="A7" s="19"/>
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="50" t="s">
+      <c r="C7" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="51" t="s">
+      <c r="D7" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="50" t="s">
+      <c r="E7" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="50" t="s">
+      <c r="F7" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="52" t="s">
+      <c r="G7" s="56" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="61" customFormat="1" ht="14.25">
-      <c r="A8" s="65"/>
-      <c r="B8" s="66">
+    <row r="8" spans="1:7" s="65" customFormat="1" ht="13.8">
+      <c r="A8" s="69"/>
+      <c r="B8" s="70">
         <v>1</v>
       </c>
-      <c r="C8" s="67" t="str">
+      <c r="C8" s="71" t="str">
         <f>Samples!B4</f>
         <v>CR100 - Export to excel</v>
       </c>
-      <c r="D8" s="68">
+      <c r="D8" s="72">
         <f>Samples!B6</f>
-        <v>3</v>
-      </c>
-      <c r="E8" s="67">
+        <v>4</v>
+      </c>
+      <c r="E8" s="71">
         <f>Samples!B7</f>
         <v>0</v>
       </c>
-      <c r="F8" s="67">
+      <c r="F8" s="71">
         <f>Samples!D6</f>
         <v>0</v>
       </c>
-      <c r="G8" s="68">
+      <c r="G8" s="72">
         <f>Samples!D7</f>
-        <v>-9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="14.25">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="13.8">
       <c r="A9" s="19"/>
       <c r="B9" s="32"/>
       <c r="C9" s="31"/>
-      <c r="D9" s="70"/>
+      <c r="D9" s="74"/>
       <c r="E9" s="30"/>
       <c r="F9" s="30"/>
       <c r="G9" s="33"/>
     </row>
-    <row r="10" spans="1:7" ht="14.25">
+    <row r="10" spans="1:7" ht="13.8">
       <c r="A10" s="19"/>
-      <c r="B10" s="53"/>
-      <c r="C10" s="54" t="s">
+      <c r="B10" s="57"/>
+      <c r="C10" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="55">
+      <c r="D10" s="59">
         <f>SUM(D6:D9)</f>
-        <v>3</v>
-      </c>
-      <c r="E10" s="55">
+        <v>4</v>
+      </c>
+      <c r="E10" s="59">
         <f>SUM(E6:E9)</f>
         <v>0</v>
       </c>
-      <c r="F10" s="55">
+      <c r="F10" s="59">
         <f>SUM(F6:F9)</f>
         <v>0</v>
       </c>
-      <c r="G10" s="56">
+      <c r="G10" s="60">
         <f>SUM(G6:G9)</f>
-        <v>-9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="14.25">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="13.8">
       <c r="A11" s="19"/>
       <c r="B11" s="20"/>
       <c r="C11" s="19"/>
@@ -2808,7 +3104,7 @@
       <c r="F11" s="22"/>
       <c r="G11" s="22"/>
     </row>
-    <row r="12" spans="1:7" ht="14.25">
+    <row r="12" spans="1:7" ht="13.8">
       <c r="A12" s="19"/>
       <c r="B12" s="19"/>
       <c r="C12" s="19" t="s">
@@ -2817,14 +3113,14 @@
       <c r="D12" s="19"/>
       <c r="E12" s="23">
         <f>(D10+E10)*100/G10</f>
-        <v>-33.333333333333336</v>
+        <v>-50</v>
       </c>
       <c r="F12" s="19" t="s">
         <v>23</v>
       </c>
       <c r="G12" s="24"/>
     </row>
-    <row r="13" spans="1:7" ht="14.25">
+    <row r="13" spans="1:7" ht="13.8">
       <c r="A13" s="19"/>
       <c r="B13" s="19"/>
       <c r="C13" s="19" t="s">
@@ -2833,7 +3129,7 @@
       <c r="D13" s="19"/>
       <c r="E13" s="23">
         <f>D10*100/G10</f>
-        <v>-33.333333333333336</v>
+        <v>-50</v>
       </c>
       <c r="F13" s="19" t="s">
         <v>23</v>

</xml_diff>